<commit_message>
Changes made in repair and tyre models and routes
</commit_message>
<xml_diff>
--- a/lr.xlsx
+++ b/lr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S.no</t>
   </si>
@@ -47,27 +47,6 @@
   </si>
   <si>
     <t>Unloading Charges</t>
-  </si>
-  <si>
-    <t>12-05-2000</t>
-  </si>
-  <si>
-    <t>Siliguri</t>
-  </si>
-  <si>
-    <t>Gangtok</t>
-  </si>
-  <si>
-    <t>3523</t>
-  </si>
-  <si>
-    <t>KRISHNA COMPANY</t>
-  </si>
-  <si>
-    <t>KRIS COMPANY</t>
-  </si>
-  <si>
-    <t>KRIS CANY</t>
   </si>
 </sst>
 </file>
@@ -448,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="10" customWidth="1"/>
@@ -496,193 +475,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>12824</v>
-      </c>
-      <c r="H2">
-        <v>84</v>
-      </c>
-      <c r="I2">
-        <v>121256</v>
-      </c>
-      <c r="J2">
-        <v>123434</v>
-      </c>
-      <c r="K2">
-        <v>193.2</v>
-      </c>
-      <c r="L2">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>12824</v>
-      </c>
-      <c r="H3">
-        <v>84</v>
-      </c>
-      <c r="I3">
-        <v>121256</v>
-      </c>
-      <c r="J3">
-        <v>123434</v>
-      </c>
-      <c r="K3">
-        <v>193.2</v>
-      </c>
-      <c r="L3">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>12824</v>
-      </c>
-      <c r="H4">
-        <v>84</v>
-      </c>
-      <c r="I4">
-        <v>121256</v>
-      </c>
-      <c r="J4">
-        <v>123434</v>
-      </c>
-      <c r="K4">
-        <v>193.2</v>
-      </c>
-      <c r="L4">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>12824</v>
-      </c>
-      <c r="H5">
-        <v>84</v>
-      </c>
-      <c r="I5">
-        <v>121256</v>
-      </c>
-      <c r="J5">
-        <v>123434</v>
-      </c>
-      <c r="K5">
-        <v>193.2</v>
-      </c>
-      <c r="L5">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6">
-        <v>12824</v>
-      </c>
-      <c r="H6">
-        <v>84</v>
-      </c>
-      <c r="I6">
-        <v>121256</v>
-      </c>
-      <c r="J6">
-        <v>123434</v>
-      </c>
-      <c r="K6">
-        <v>193.2</v>
-      </c>
-      <c r="L6">
-        <v>820</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>